<commit_message>
#12289 and #12288 feedback done
</commit_message>
<xml_diff>
--- a/OutputReports/DHIS2 Reports/HTML Reports/Maharashtra/RCH Reports/#12289 Condom Users Report/8. Condom Users.xlsx
+++ b/OutputReports/DHIS2 Reports/HTML Reports/Maharashtra/RCH Reports/#12289 Condom Users Report/8. Condom Users.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19860" windowHeight="7950"/>
+    <workbookView windowWidth="23895" windowHeight="10335"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54">
   <si>
     <t>State Family Welfare Bureau,Pune</t>
   </si>
@@ -79,52 +79,103 @@
     <t>DH - Rural</t>
   </si>
   <si>
+    <t>gwKt4p6FHVC</t>
+  </si>
+  <si>
     <t>GH Group</t>
   </si>
   <si>
+    <t>ST9J0WWZRQI</t>
+  </si>
+  <si>
     <t>MCL Group</t>
   </si>
   <si>
+    <t>gF8yOGpymoX</t>
+  </si>
+  <si>
     <t>RH Group</t>
   </si>
   <si>
+    <t>I5y0Khag603</t>
+  </si>
+  <si>
     <t>SDH 100 Group</t>
   </si>
   <si>
+    <t>WucfWEzRAJ6</t>
+  </si>
+  <si>
     <t>SDH 50 Group</t>
   </si>
   <si>
+    <t>wqezxH4KlLF</t>
+  </si>
+  <si>
     <t>WH Group</t>
   </si>
   <si>
+    <t>l5TS6kLRJOI</t>
+  </si>
+  <si>
     <t>PHC - Rural</t>
   </si>
   <si>
+    <t>YOLBalOi30g</t>
+  </si>
+  <si>
     <t>SC Group</t>
   </si>
   <si>
+    <t>bYeMmLxh8Xs</t>
+  </si>
+  <si>
     <t>Cantonment group</t>
   </si>
   <si>
+    <t>oamujLzycVd</t>
+  </si>
+  <si>
     <t>Rural Facility group</t>
   </si>
   <si>
+    <t>B2Rs7d7N5BW</t>
+  </si>
+  <si>
     <t>2. Use following groups for Corporation total fields:</t>
   </si>
   <si>
     <t>UPHC Group</t>
   </si>
   <si>
+    <t>M8aNrEBmf4K</t>
+  </si>
+  <si>
     <t>UCHC Group</t>
   </si>
   <si>
+    <t>UAnG4KYJ8LH</t>
+  </si>
+  <si>
     <t>USDH Group</t>
   </si>
   <si>
+    <t>USYXisAI852</t>
+  </si>
+  <si>
     <t>UDH Group</t>
   </si>
   <si>
+    <t>s1B0HZ22VBp</t>
+  </si>
+  <si>
     <t>Corporation Group</t>
+  </si>
+  <si>
+    <t>YBJEhiPcxsw</t>
+  </si>
+  <si>
+    <t>bMuNJdhKC3M</t>
   </si>
 </sst>
 </file>
@@ -132,12 +183,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,10 +237,38 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="10.5"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -200,24 +279,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,112 +347,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="37">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,187 +426,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -617,15 +662,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -637,6 +673,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -674,6 +734,15 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -690,181 +759,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -902,10 +947,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1233,10 +1281,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1296,8 +1344,8 @@
         <v>6</v>
       </c>
       <c r="H3" s="6"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:10">
       <c r="A4" s="2"/>
@@ -1320,10 +1368,10 @@
       <c r="H4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="16" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1348,10 +1396,10 @@
       <c r="H5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="17" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1360,89 +1408,142 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="4:4">
+    <row r="9" spans="4:5">
       <c r="D9" s="12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="4:4">
+      <c r="E9" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5">
       <c r="D10" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="4:4">
+        <v>22</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5">
       <c r="D11" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="4:4">
+        <v>24</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="4:5">
       <c r="D12" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="4:4">
+        <v>26</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="4:5">
       <c r="D13" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="4:4">
+        <v>28</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="4:5">
       <c r="D14" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="4:4">
+        <v>30</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="4:5">
       <c r="D15" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="4:4">
+        <v>32</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="4:5">
       <c r="D16" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4">
+        <v>34</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5">
       <c r="D17" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4">
+        <v>36</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5">
       <c r="D18" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4">
+        <v>38</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5">
       <c r="D19" s="12" t="s">
-        <v>30</v>
+        <v>40</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="21" ht="45" spans="4:4">
       <c r="D21" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="4:4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5">
       <c r="D22" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="4:4">
+        <v>43</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5">
       <c r="D23" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="4:4">
+        <v>45</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5">
       <c r="D24" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="4:4">
+        <v>47</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5">
       <c r="D25" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="4:4">
+        <v>49</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="4:5">
       <c r="D26" s="12" t="s">
-        <v>36</v>
+        <v>51</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
+      <c r="E27" s="13" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>